<commit_message>
multiline test with refs
</commit_message>
<xml_diff>
--- a/seedtable-test/test-resources/seedtable_example.xlsx
+++ b/seedtable-test/test-resources/seedtable_example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="14800" windowHeight="8020" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="foos" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="yamls" sheetId="1" r:id="rId5"/>
     <sheet name="datetimes" sheetId="5" r:id="rId6"/>
     <sheet name="multilines" sheetId="7" r:id="rId7"/>
+    <sheet name="multiline_refs" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -169,6 +170,14 @@
   <si>
     <t>line1
 line2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>multi</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2282,8 +2291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2336,4 +2345,55 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <f>VLOOKUP(A3,multilines!$A$3:$C$999,3)</f>
+        <v>line1_x000D_line2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="98" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="str">
+        <f>VLOOKUP(A4,multilines!$A$3:$C$999,3)</f>
+        <v>line1_x000D_line2_x000D__x000D_line4_x000D__x000D__x000D_line7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="126" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <f>VLOOKUP(A5,multilines!$A$3:$C$999,3)</f>
+        <v>_x000D_line2_x000D_line3_x000D__x000D_line5_x000D__x000D__x000D_line8_x000D_</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>